<commit_message>
Exercício proposto - Ajustes
</commit_message>
<xml_diff>
--- a/módulo 04/exercicio-proposto-formas-e-mais.xlsx
+++ b/módulo 04/exercicio-proposto-formas-e-mais.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="30">
   <si>
     <t>MENU</t>
   </si>
@@ -116,25 +116,7 @@
     <t>Estoques!A1</t>
   </si>
   <si>
-    <t>seg</t>
-  </si>
-  <si>
-    <t>ter</t>
-  </si>
-  <si>
-    <t>qua</t>
-  </si>
-  <si>
-    <t>qui</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>sáb</t>
-  </si>
-  <si>
-    <t>dom</t>
+    <t>Preencher automático: põe o valor na célula/clica em preencher/série/escolhe os parametros</t>
   </si>
 </sst>
 </file>
@@ -492,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -647,35 +629,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1087,7 +1072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:B8"/>
     </sheetView>
   </sheetViews>
@@ -1102,12 +1087,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2"/>
@@ -1125,7 +1110,7 @@
       <c r="O2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="54" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="4"/>
@@ -1143,7 +1128,7 @@
       <c r="O3" s="5"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="60"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1159,73 +1144,73 @@
       <c r="O4" s="5"/>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="52" t="s">
+      <c r="G5" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="60"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="52"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="52"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
+      <c r="L6" s="55"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="52"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="5"/>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="56"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="56"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="5"/>
@@ -1518,7 +1503,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -1553,7 +1538,7 @@
       </c>
     </row>
     <row r="3" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="59" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="21"/>
@@ -1571,35 +1556,35 @@
       <c r="O3" s="22"/>
     </row>
     <row r="4" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="58"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="21"/>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="56" t="s">
+      <c r="F4" s="58"/>
+      <c r="G4" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="57"/>
-      <c r="I4" s="56" t="s">
+      <c r="H4" s="58"/>
+      <c r="I4" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="57"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="57"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="58"/>
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="21"/>
-      <c r="D5" s="55"/>
+      <c r="D5" s="61"/>
       <c r="E5" s="26" t="s">
         <v>8</v>
       </c>
@@ -1625,10 +1610,10 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="60"/>
+      <c r="B6" s="54"/>
       <c r="C6" s="21"/>
-      <c r="D6" s="34" t="s">
-        <v>29</v>
+      <c r="D6" s="34">
+        <v>43647</v>
       </c>
       <c r="E6" s="28"/>
       <c r="F6" s="29"/>
@@ -1643,12 +1628,12 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="21"/>
-      <c r="D7" s="35" t="s">
-        <v>30</v>
+      <c r="D7" s="35">
+        <v>43648</v>
       </c>
       <c r="E7" s="30"/>
       <c r="F7" s="31"/>
@@ -1663,10 +1648,10 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="21"/>
-      <c r="D8" s="35" t="s">
-        <v>31</v>
+      <c r="D8" s="35">
+        <v>43649</v>
       </c>
       <c r="E8" s="30"/>
       <c r="F8" s="31"/>
@@ -1683,8 +1668,8 @@
     <row r="9" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18"/>
       <c r="C9" s="21"/>
-      <c r="D9" s="35" t="s">
-        <v>32</v>
+      <c r="D9" s="35">
+        <v>43650</v>
       </c>
       <c r="E9" s="30"/>
       <c r="F9" s="31"/>
@@ -1701,8 +1686,8 @@
     <row r="10" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="21"/>
-      <c r="D10" s="35" t="s">
-        <v>33</v>
+      <c r="D10" s="35">
+        <v>43651</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="31"/>
@@ -1719,8 +1704,8 @@
     <row r="11" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="19"/>
       <c r="C11" s="21"/>
-      <c r="D11" s="35" t="s">
-        <v>34</v>
+      <c r="D11" s="35">
+        <v>43652</v>
       </c>
       <c r="E11" s="30"/>
       <c r="F11" s="31"/>
@@ -1737,8 +1722,8 @@
     <row r="12" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
       <c r="C12" s="21"/>
-      <c r="D12" s="35" t="s">
-        <v>35</v>
+      <c r="D12" s="35">
+        <v>43653</v>
       </c>
       <c r="E12" s="30"/>
       <c r="F12" s="31"/>
@@ -1755,8 +1740,8 @@
     <row r="13" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
       <c r="C13" s="21"/>
-      <c r="D13" s="35" t="s">
-        <v>29</v>
+      <c r="D13" s="35">
+        <v>43654</v>
       </c>
       <c r="E13" s="30"/>
       <c r="F13" s="31"/>
@@ -1773,8 +1758,8 @@
     <row r="14" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
       <c r="C14" s="21"/>
-      <c r="D14" s="35" t="s">
-        <v>30</v>
+      <c r="D14" s="35">
+        <v>43655</v>
       </c>
       <c r="E14" s="30"/>
       <c r="F14" s="31"/>
@@ -1791,8 +1776,8 @@
     <row r="15" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="16"/>
       <c r="C15" s="21"/>
-      <c r="D15" s="35" t="s">
-        <v>31</v>
+      <c r="D15" s="35">
+        <v>43656</v>
       </c>
       <c r="E15" s="30"/>
       <c r="F15" s="31"/>
@@ -1809,8 +1794,8 @@
     <row r="16" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="16"/>
       <c r="C16" s="21"/>
-      <c r="D16" s="35" t="s">
-        <v>32</v>
+      <c r="D16" s="35">
+        <v>43657</v>
       </c>
       <c r="E16" s="30"/>
       <c r="F16" s="31"/>
@@ -1827,8 +1812,8 @@
     <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="16"/>
       <c r="C17" s="21"/>
-      <c r="D17" s="35" t="s">
-        <v>33</v>
+      <c r="D17" s="35">
+        <v>43658</v>
       </c>
       <c r="E17" s="30"/>
       <c r="F17" s="31"/>
@@ -1845,8 +1830,8 @@
     <row r="18" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="16"/>
       <c r="C18" s="21"/>
-      <c r="D18" s="35" t="s">
-        <v>34</v>
+      <c r="D18" s="35">
+        <v>43659</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="31"/>
@@ -1863,8 +1848,8 @@
     <row r="19" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="16"/>
       <c r="C19" s="21"/>
-      <c r="D19" s="35" t="s">
-        <v>35</v>
+      <c r="D19" s="35">
+        <v>43660</v>
       </c>
       <c r="E19" s="30"/>
       <c r="F19" s="31"/>
@@ -1881,8 +1866,8 @@
     <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="16"/>
       <c r="C20" s="21"/>
-      <c r="D20" s="35" t="s">
-        <v>29</v>
+      <c r="D20" s="35">
+        <v>43661</v>
       </c>
       <c r="E20" s="30"/>
       <c r="F20" s="31"/>
@@ -1899,8 +1884,8 @@
     <row r="21" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="16"/>
       <c r="C21" s="21"/>
-      <c r="D21" s="35" t="s">
-        <v>30</v>
+      <c r="D21" s="35">
+        <v>43662</v>
       </c>
       <c r="E21" s="30"/>
       <c r="F21" s="31"/>
@@ -1917,8 +1902,8 @@
     <row r="22" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="16"/>
       <c r="C22" s="21"/>
-      <c r="D22" s="35" t="s">
-        <v>31</v>
+      <c r="D22" s="35">
+        <v>43663</v>
       </c>
       <c r="E22" s="30"/>
       <c r="F22" s="31"/>
@@ -1935,8 +1920,8 @@
     <row r="23" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="16"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="35" t="s">
-        <v>32</v>
+      <c r="D23" s="35">
+        <v>43664</v>
       </c>
       <c r="E23" s="30"/>
       <c r="F23" s="31"/>
@@ -1953,8 +1938,8 @@
     <row r="24" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="16"/>
       <c r="C24" s="21"/>
-      <c r="D24" s="35" t="s">
-        <v>33</v>
+      <c r="D24" s="35">
+        <v>43665</v>
       </c>
       <c r="E24" s="30"/>
       <c r="F24" s="31"/>
@@ -1971,8 +1956,8 @@
     <row r="25" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="16"/>
       <c r="C25" s="21"/>
-      <c r="D25" s="35" t="s">
-        <v>34</v>
+      <c r="D25" s="35">
+        <v>43666</v>
       </c>
       <c r="E25" s="30"/>
       <c r="F25" s="31"/>
@@ -1989,8 +1974,8 @@
     <row r="26" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="16"/>
       <c r="C26" s="21"/>
-      <c r="D26" s="36" t="s">
-        <v>35</v>
+      <c r="D26" s="36">
+        <v>43667</v>
       </c>
       <c r="E26" s="32"/>
       <c r="F26" s="33"/>
@@ -2024,15 +2009,15 @@
     <row r="29" spans="2:15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" location="Menu!A1" display="MENU"/>
@@ -2040,6 +2025,7 @@
     <hyperlink ref="B7:B8" location="Relatório!A1" display="Relatório"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2060,7 +2046,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="53" t="s">
         <v>28</v>
       </c>
     </row>
@@ -2085,7 +2071,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="54" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="21"/>
@@ -2103,7 +2089,7 @@
       <c r="O3" s="22"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="60"/>
+      <c r="B4" s="54"/>
       <c r="C4" s="21"/>
       <c r="D4" s="37"/>
       <c r="E4" s="37"/>
@@ -2119,7 +2105,7 @@
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="59" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="21"/>
@@ -2137,7 +2123,7 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="58"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="21"/>
       <c r="D6" s="37"/>
       <c r="E6" s="37"/>
@@ -2153,7 +2139,7 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="54" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="21"/>
@@ -2171,7 +2157,7 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="60"/>
+      <c r="B8" s="54"/>
       <c r="C8" s="21"/>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
@@ -2511,7 +2497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2524,10 +2512,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
+      <c r="A1" s="53"/>
     </row>
     <row r="2" spans="1:15" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="61"/>
+      <c r="A2" s="53"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="50" t="s">
@@ -2550,7 +2538,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="54" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="21"/>
@@ -2568,7 +2556,7 @@
       <c r="O4" s="22"/>
     </row>
     <row r="5" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="60"/>
+      <c r="B5" s="54"/>
       <c r="C5" s="21"/>
       <c r="D5" s="37"/>
       <c r="E5" s="38" t="s">
@@ -2588,7 +2576,7 @@
       <c r="O5" s="22"/>
     </row>
     <row r="6" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="54" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="21"/>
@@ -2614,7 +2602,7 @@
       <c r="K6" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="49" t="s">
+      <c r="L6" s="62" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="37"/>
@@ -2622,7 +2610,7 @@
       <c r="O6" s="22"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="60"/>
+      <c r="B7" s="54"/>
       <c r="C7" s="21"/>
       <c r="D7" s="37"/>
       <c r="E7" s="40" t="s">
@@ -2640,7 +2628,7 @@
       <c r="O7" s="22"/>
     </row>
     <row r="8" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="58" t="s">
+      <c r="B8" s="59" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="21"/>
@@ -2660,7 +2648,7 @@
       <c r="O8" s="22"/>
     </row>
     <row r="9" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="58"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="21"/>
       <c r="D9" s="37"/>
       <c r="E9" s="45" t="s">
@@ -2981,7 +2969,11 @@
       <c r="N28" s="23"/>
       <c r="O28" s="24"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="3">

</xml_diff>